<commit_message>
CADE - Archivo Portales Contrasena
Se cambia la contrasena en la cade sanborns para que se pueda consulta
por parte de los programados por si se requiere que entre a revisar.
</commit_message>
<xml_diff>
--- a/Credenciales - Portales.xlsx
+++ b/Credenciales - Portales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CapacitacionDesarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D25ED7AC-28AB-4192-8ED2-9BE529C68A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45145810-D94F-4404-A004-CE74AC9A7A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C30447A1-1B82-468F-95A4-B687C3F712A1}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>http://proveedores.sanborns.com.mx</t>
   </si>
   <si>
-    <t>Intermex202111</t>
-  </si>
-  <si>
     <t>https://rllogin.wal-mart.com/rl_security/rl_logon.aspx</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Intermex.1123</t>
+  </si>
+  <si>
+    <t>Intermex202201</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -577,13 +577,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,13 +594,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>600787</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,13 +628,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -645,13 +645,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,13 +662,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -679,13 +679,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,13 +696,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,13 +713,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>600787</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,13 +747,13 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -764,13 +764,13 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,13 +781,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,16 +815,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,13 +835,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -852,13 +852,13 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,13 +869,13 @@
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,13 +886,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>600787</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -920,13 +920,13 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -937,13 +937,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>